<commit_message>
Conduct S4 tests for tradidional Graphql and traditional Graphql with selected fields
</commit_message>
<xml_diff>
--- a/Wyniki 3/S3.xlsx
+++ b/Wyniki 3/S3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kacpe\OneDrive\Pulpit\Projekty\Praca magisterska\Wyniki 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524AA1EA-6C92-413A-922E-47DA964E0528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAF8300-0C53-40F8-99AE-EDD027EF94DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-2340" windowWidth="25820" windowHeight="15500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REST" sheetId="1" r:id="rId1"/>
@@ -7241,7 +7241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491B2463-697C-4FC5-A88C-76F5DBC70B85}">
   <dimension ref="E7:L50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -8223,7 +8223,7 @@
   <dimension ref="E7:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="R52" sqref="R52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>